<commit_message>
rated moles, for real
</commit_message>
<xml_diff>
--- a/task_1.xlsx
+++ b/task_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/srde_itu_dk/Documents/II/FYP/p02/fyp2022p02gj2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alteafogh/Desktop/python/fyp/fyp2022p02gj2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{B8C53454-4402-2443-9063-75CDDFCEBA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E6F4B65-9FE8-4BF8-B3B9-8C7248DB883E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC195AFE-4A53-9B4A-8CA4-4745DF61183F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -834,23 +831,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -858,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>153</v>
       </c>
@@ -875,7 +872,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -891,8 +888,11 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -908,8 +908,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -925,8 +928,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -942,8 +948,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -959,8 +968,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -976,8 +988,11 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -993,8 +1008,11 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1010,8 +1028,11 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1027,8 +1048,11 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1044,8 +1068,11 @@
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1061,8 +1088,11 @@
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1078,8 +1108,11 @@
       <c r="E15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1095,8 +1128,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1112,8 +1148,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1129,8 +1168,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1146,8 +1188,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1163,8 +1208,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1180,8 +1228,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1197,8 +1248,11 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1214,8 +1268,11 @@
       <c r="E23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1231,8 +1288,11 @@
       <c r="E24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1248,8 +1308,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1265,8 +1328,11 @@
       <c r="E26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1282,8 +1348,11 @@
       <c r="E27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1299,8 +1368,11 @@
       <c r="E28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1316,8 +1388,11 @@
       <c r="E29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1333,8 +1408,11 @@
       <c r="E30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1350,8 +1428,11 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1367,8 +1448,11 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1384,8 +1468,11 @@
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1401,8 +1488,11 @@
       <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1418,8 +1508,11 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1435,8 +1528,11 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1452,8 +1548,11 @@
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1469,8 +1568,11 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1486,8 +1588,11 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1503,8 +1608,11 @@
       <c r="E40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1520,8 +1628,11 @@
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1537,8 +1648,11 @@
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1554,8 +1668,11 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1571,8 +1688,11 @@
       <c r="E44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1588,8 +1708,11 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1605,8 +1728,11 @@
       <c r="E46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1622,8 +1748,11 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1639,8 +1768,11 @@
       <c r="E48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1656,8 +1788,11 @@
       <c r="E49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1673,8 +1808,11 @@
       <c r="E50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1690,8 +1828,11 @@
       <c r="E51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1707,8 +1848,11 @@
       <c r="E52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1724,8 +1868,11 @@
       <c r="E53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1741,8 +1888,11 @@
       <c r="E54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1758,8 +1908,11 @@
       <c r="E55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1775,8 +1928,11 @@
       <c r="E56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1792,8 +1948,11 @@
       <c r="E57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1809,8 +1968,11 @@
       <c r="E58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1826,8 +1988,11 @@
       <c r="E59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1843,8 +2008,11 @@
       <c r="E60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1860,8 +2028,11 @@
       <c r="E61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1877,8 +2048,11 @@
       <c r="E62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1894,8 +2068,11 @@
       <c r="E63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1911,8 +2088,11 @@
       <c r="E64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1928,8 +2108,11 @@
       <c r="E65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1945,8 +2128,11 @@
       <c r="E66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1962,8 +2148,11 @@
       <c r="E67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1979,8 +2168,11 @@
       <c r="E68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1996,8 +2188,11 @@
       <c r="E69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2013,8 +2208,11 @@
       <c r="E70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2030,8 +2228,11 @@
       <c r="E71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2047,8 +2248,11 @@
       <c r="E72">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -2064,8 +2268,11 @@
       <c r="E73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -2081,8 +2288,11 @@
       <c r="E74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -2098,8 +2308,11 @@
       <c r="E75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -2115,8 +2328,11 @@
       <c r="E76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2132,8 +2348,11 @@
       <c r="E77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2149,8 +2368,11 @@
       <c r="E78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -2166,8 +2388,11 @@
       <c r="E79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2183,8 +2408,11 @@
       <c r="E80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -2200,8 +2428,11 @@
       <c r="E81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -2217,8 +2448,11 @@
       <c r="E82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -2234,8 +2468,11 @@
       <c r="E83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -2251,8 +2488,11 @@
       <c r="E84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -2268,8 +2508,11 @@
       <c r="E85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -2285,8 +2528,11 @@
       <c r="E86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -2302,8 +2548,11 @@
       <c r="E87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -2319,8 +2568,11 @@
       <c r="E88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -2336,8 +2588,11 @@
       <c r="E89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -2353,8 +2608,11 @@
       <c r="E90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -2370,8 +2628,11 @@
       <c r="E91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2387,8 +2648,11 @@
       <c r="E92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -2404,8 +2668,11 @@
       <c r="E93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -2421,8 +2688,11 @@
       <c r="E94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -2438,8 +2708,11 @@
       <c r="E95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -2455,8 +2728,11 @@
       <c r="E96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -2472,8 +2748,11 @@
       <c r="E97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -2489,8 +2768,11 @@
       <c r="E98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -2506,8 +2788,11 @@
       <c r="E99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -2523,8 +2808,11 @@
       <c r="E100">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -2540,8 +2828,11 @@
       <c r="E101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -2557,8 +2848,11 @@
       <c r="E102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -2574,8 +2868,11 @@
       <c r="E103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -2591,8 +2888,11 @@
       <c r="E104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -2608,8 +2908,11 @@
       <c r="E105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -2625,8 +2928,11 @@
       <c r="E106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -2642,8 +2948,11 @@
       <c r="E107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -2659,8 +2968,11 @@
       <c r="E108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2676,8 +2988,11 @@
       <c r="E109">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -2693,8 +3008,11 @@
       <c r="E110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -2710,8 +3028,11 @@
       <c r="E111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2727,8 +3048,11 @@
       <c r="E112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -2744,8 +3068,11 @@
       <c r="E113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -2761,8 +3088,11 @@
       <c r="E114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -2778,8 +3108,11 @@
       <c r="E115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -2795,8 +3128,11 @@
       <c r="E116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -2812,8 +3148,11 @@
       <c r="E117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -2829,8 +3168,11 @@
       <c r="E118">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -2846,8 +3188,11 @@
       <c r="E119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -2863,8 +3208,11 @@
       <c r="E120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -2880,8 +3228,11 @@
       <c r="E121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -2897,8 +3248,11 @@
       <c r="E122">
         <v>2</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -2914,8 +3268,11 @@
       <c r="E123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -2931,8 +3288,11 @@
       <c r="E124">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -2948,8 +3308,11 @@
       <c r="E125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -2965,8 +3328,11 @@
       <c r="E126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -2982,8 +3348,11 @@
       <c r="E127">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -2999,8 +3368,11 @@
       <c r="E128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -3016,8 +3388,11 @@
       <c r="E129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -3033,8 +3408,11 @@
       <c r="E130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -3050,8 +3428,11 @@
       <c r="E131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -3067,8 +3448,11 @@
       <c r="E132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -3084,8 +3468,11 @@
       <c r="E133">
         <v>2</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -3101,8 +3488,11 @@
       <c r="E134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -3118,8 +3508,11 @@
       <c r="E135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -3135,8 +3528,11 @@
       <c r="E136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -3152,8 +3548,11 @@
       <c r="E137">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -3169,8 +3568,11 @@
       <c r="E138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -3186,8 +3588,11 @@
       <c r="E139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -3203,8 +3608,11 @@
       <c r="E140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -3220,8 +3628,11 @@
       <c r="E141">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
@@ -3237,8 +3648,11 @@
       <c r="E142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
@@ -3254,8 +3668,11 @@
       <c r="E143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -3271,8 +3688,11 @@
       <c r="E144">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -3288,8 +3708,11 @@
       <c r="E145">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -3305,8 +3728,11 @@
       <c r="E146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -3322,8 +3748,11 @@
       <c r="E147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>146</v>
       </c>
@@ -3339,8 +3768,11 @@
       <c r="E148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>147</v>
       </c>
@@ -3356,8 +3788,11 @@
       <c r="E149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -3373,8 +3808,11 @@
       <c r="E150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -3390,8 +3828,11 @@
       <c r="E151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -3407,8 +3848,11 @@
       <c r="E152">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -3424,8 +3868,11 @@
       <c r="E153">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B154" s="1"/>
     </row>
   </sheetData>

</xml_diff>